<commit_message>
Live Code Order Improved
</commit_message>
<xml_diff>
--- a/Current Work/Live Code/EURJPY_Dynamic.xlsx
+++ b/Current Work/Live Code/EURJPY_Dynamic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Techincal Analysis Program\MT5\Current Work\Live Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33938DE3-CA12-4DD4-9A33-89A852FB0582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD0DB31-CEDD-4383-AADC-98B6AF97C684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -143,7 +143,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N633"/>
+  <dimension ref="A1:N634"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A606" workbookViewId="0">
       <selection activeCell="I634" sqref="I634"/>
@@ -28316,6 +28316,12 @@
         <v>19</v>
       </c>
     </row>
+    <row r="634" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I634">
+        <f>SUM(I2:I633)</f>
+        <v>23423.805736673494</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>